<commit_message>
Added ability to remove food from ration.
</commit_message>
<xml_diff>
--- a/RightFood/FoodList.xlsx
+++ b/RightFood/FoodList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>mI * 10000</t>
+  </si>
+  <si>
+    <t>Апельсиновый сок</t>
+  </si>
+  <si>
+    <t>Сыр Рикотта 7-9%</t>
+  </si>
+  <si>
+    <t>Сыр Моцарелла</t>
   </si>
 </sst>
 </file>
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +483,7 @@
     <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" style="1" customWidth="1"/>
@@ -486,7 +495,8 @@
     <col min="17" max="17" width="21.140625" style="1" customWidth="1"/>
     <col min="18" max="18" width="15.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="9.140625" style="1"/>
-    <col min="20" max="22" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.85546875" style="1" customWidth="1"/>
     <col min="24" max="25" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -494,7 +504,7 @@
     <col min="28" max="28" width="9.140625" style="1"/>
     <col min="29" max="29" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13.140625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -619,7 +629,7 @@
         <v>68000</v>
       </c>
       <c r="H2" s="1">
-        <v>290000</v>
+        <v>210000</v>
       </c>
       <c r="I2" s="1">
         <v>340000</v>
@@ -717,7 +727,7 @@
         <v>176000</v>
       </c>
       <c r="H3" s="1">
-        <v>380000</v>
+        <v>280000</v>
       </c>
       <c r="I3" s="1">
         <v>320000</v>
@@ -790,10 +800,305 @@
       </c>
       <c r="AF3" s="1">
         <v>1325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>104000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>11000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>430000</v>
+      </c>
+      <c r="I4" s="1">
+        <v>900000</v>
+      </c>
+      <c r="J4" s="1">
+        <v>300000</v>
+      </c>
+      <c r="K4" s="1">
+        <v>400</v>
+      </c>
+      <c r="L4" s="1">
+        <v>190</v>
+      </c>
+      <c r="M4" s="1">
+        <v>400000</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>300000</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>40</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="U4" s="1">
+        <v>200</v>
+      </c>
+      <c r="V4" s="1">
+        <v>11000</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1">
+        <v>200000</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>11000</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>44</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>17000</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>50</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>100</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1">
+        <v>140</v>
+      </c>
+      <c r="D5" s="1">
+        <v>114000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>79100</v>
+      </c>
+      <c r="F5" s="1">
+        <v>51000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>70000</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1250000</v>
+      </c>
+      <c r="I5" s="1">
+        <v>210000</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1850000</v>
+      </c>
+      <c r="K5" s="1">
+        <v>78</v>
+      </c>
+      <c r="L5" s="1">
+        <v>242</v>
+      </c>
+      <c r="M5" s="1">
+        <v>200000</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>230000</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2900</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="S5" s="1">
+        <v>70</v>
+      </c>
+      <c r="T5" s="1">
+        <v>7000</v>
+      </c>
+      <c r="U5" s="1">
+        <v>440</v>
+      </c>
+      <c r="V5" s="1">
+        <v>272000</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>125000</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>15000</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>34</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>183000</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>1340</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>16700</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>99000</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1">
+        <v>301</v>
+      </c>
+      <c r="D6" s="1">
+        <v>246000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>197200</v>
+      </c>
+      <c r="F6" s="1">
+        <v>64000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>166000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2540000</v>
+      </c>
+      <c r="I6" s="1">
+        <v>590000</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3480000</v>
+      </c>
+      <c r="K6" s="1">
+        <v>144</v>
+      </c>
+      <c r="L6" s="1">
+        <v>415</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1110000</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>270000</v>
+      </c>
+      <c r="P6" s="1">
+        <v>18200</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>4000</v>
+      </c>
+      <c r="S6" s="1">
+        <v>430</v>
+      </c>
+      <c r="T6" s="1">
+        <v>13000</v>
+      </c>
+      <c r="U6" s="1">
+        <v>230</v>
+      </c>
+      <c r="V6" s="1">
+        <v>716000</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
+        <v>131000</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>29000</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>34</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>537000</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>3610</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>26800</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>682000</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Database of products was updated.
</commit_message>
<xml_diff>
--- a/RightFood/FoodList.xlsx
+++ b/RightFood/FoodList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>id</t>
   </si>
@@ -126,16 +126,64 @@
     <t>Сыр Рикотта 7-9%</t>
   </si>
   <si>
-    <t>Сыр Моцарелла</t>
+    <t>Сыр Моцарелла 19%</t>
+  </si>
+  <si>
+    <t>Яйца куриные</t>
+  </si>
+  <si>
+    <t>Томаты желтые</t>
+  </si>
+  <si>
+    <t>Томаты красные</t>
+  </si>
+  <si>
+    <t>Хлеб зерновой</t>
+  </si>
+  <si>
+    <t>Сыр Гран-При (brick)</t>
+  </si>
+  <si>
+    <t>Орехи Кешью</t>
+  </si>
+  <si>
+    <t>Орехи Арахис</t>
+  </si>
+  <si>
+    <t>Орехи Миндаль</t>
+  </si>
+  <si>
+    <t>Семечки тыквенные</t>
+  </si>
+  <si>
+    <t>Перец Красный сладкий</t>
+  </si>
+  <si>
+    <t>Перец Желтый сладкий</t>
+  </si>
+  <si>
+    <t>Бананы</t>
+  </si>
+  <si>
+    <t>Печень говяжья</t>
+  </si>
+  <si>
+    <t>Говядина</t>
+  </si>
+  <si>
+    <t>Печень свиная</t>
+  </si>
+  <si>
+    <t>Семга</t>
+  </si>
+  <si>
+    <t>Индейка</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -167,7 +215,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -469,43 +517,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" style="1" customWidth="1"/>
     <col min="16" max="16" width="13" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="1"/>
-    <col min="20" max="21" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" style="1" customWidth="1"/>
-    <col min="24" max="25" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="1"/>
-    <col min="29" max="29" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="7" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="10" style="1" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="6.5703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="7.7109375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.42578125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" style="1" customWidth="1"/>
+    <col min="32" max="32" width="7.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -816,7 +867,7 @@
         <v>7000</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="F4" s="1">
         <v>104000</v>
@@ -1094,6 +1145,1672 @@
       </c>
       <c r="AF6" s="1">
         <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1">
+        <v>155</v>
+      </c>
+      <c r="D7" s="1">
+        <v>126000</v>
+      </c>
+      <c r="E7" s="1">
+        <v>106100</v>
+      </c>
+      <c r="F7" s="1">
+        <v>11000</v>
+      </c>
+      <c r="G7" s="1">
+        <v>78000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1600000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>660000</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5130000</v>
+      </c>
+      <c r="K7" s="1">
+        <v>64</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1398</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1210000</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>440000</v>
+      </c>
+      <c r="P7" s="1">
+        <v>11100</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>20000</v>
+      </c>
+      <c r="S7" s="1">
+        <v>1030</v>
+      </c>
+      <c r="T7" s="1">
+        <v>3000</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1190</v>
+      </c>
+      <c r="V7" s="1">
+        <v>50000</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
+        <v>126000</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>10000</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>172000</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>1050</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>30800</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>124000</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9800</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2600</v>
+      </c>
+      <c r="F8" s="1">
+        <v>29800</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>410000</v>
+      </c>
+      <c r="J8" s="1">
+        <v>470000</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1179</v>
+      </c>
+      <c r="L8" s="1">
+        <v>110</v>
+      </c>
+      <c r="M8" s="1">
+        <v>560000</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>300000</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>9000</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <v>490</v>
+      </c>
+      <c r="V8" s="1">
+        <v>11000</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>258000</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>12000</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>101</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>36000</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>280</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>400</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>23000</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F9" s="1">
+        <v>39000</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4900000</v>
+      </c>
+      <c r="I9" s="1">
+        <v>370000</v>
+      </c>
+      <c r="J9" s="1">
+        <v>190000</v>
+      </c>
+      <c r="K9" s="1">
+        <v>594</v>
+      </c>
+      <c r="L9" s="1">
+        <v>89</v>
+      </c>
+      <c r="M9" s="1">
+        <v>800000</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>150000</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>13700</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>540</v>
+      </c>
+      <c r="T9" s="1">
+        <v>79000</v>
+      </c>
+      <c r="U9" s="1">
+        <v>270</v>
+      </c>
+      <c r="V9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
+        <v>237000</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>11000</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>59</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>24000</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>170</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>5000</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1">
+        <v>265</v>
+      </c>
+      <c r="D10" s="1">
+        <v>134000</v>
+      </c>
+      <c r="E10" s="1">
+        <v>42300</v>
+      </c>
+      <c r="F10" s="1">
+        <v>433000</v>
+      </c>
+      <c r="G10" s="1">
+        <v>205000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2790000</v>
+      </c>
+      <c r="J10" s="1">
+        <v>131000</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4042</v>
+      </c>
+      <c r="L10" s="1">
+        <v>336</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2360000</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>750000</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>100</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>370</v>
+      </c>
+      <c r="T10" s="1">
+        <v>14000</v>
+      </c>
+      <c r="U10" s="1">
+        <v>2500</v>
+      </c>
+      <c r="V10" s="1">
+        <v>103000</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1">
+        <v>230000</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>78000</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>282</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>228000</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>1700</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>32900</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>381000</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1">
+        <v>371</v>
+      </c>
+      <c r="D11" s="1">
+        <v>232000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>296800</v>
+      </c>
+      <c r="F11" s="1">
+        <v>28000</v>
+      </c>
+      <c r="G11" s="1">
+        <v>293000</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3620000</v>
+      </c>
+      <c r="I11" s="1">
+        <v>140000</v>
+      </c>
+      <c r="J11" s="1">
+        <v>351000</v>
+      </c>
+      <c r="K11" s="1">
+        <v>118</v>
+      </c>
+      <c r="L11" s="1">
+        <v>288</v>
+      </c>
+      <c r="M11" s="1">
+        <v>650000</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>200000</v>
+      </c>
+      <c r="P11" s="1">
+        <v>12600</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="S11" s="1">
+        <v>260</v>
+      </c>
+      <c r="T11" s="1">
+        <v>25000</v>
+      </c>
+      <c r="U11" s="1">
+        <v>430</v>
+      </c>
+      <c r="V11" s="1">
+        <v>674000</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>136000</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>24000</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>451000</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>2600</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>14500</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>560000</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="1">
+        <v>553</v>
+      </c>
+      <c r="D12" s="1">
+        <v>182000</v>
+      </c>
+      <c r="E12" s="1">
+        <v>438500</v>
+      </c>
+      <c r="F12" s="1">
+        <v>302000</v>
+      </c>
+      <c r="G12" s="1">
+        <v>62000</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>4230000</v>
+      </c>
+      <c r="J12" s="1">
+        <v>580000</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1062</v>
+      </c>
+      <c r="L12" s="1">
+        <v>864</v>
+      </c>
+      <c r="M12" s="1">
+        <v>4170000</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>250000</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>500</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>900</v>
+      </c>
+      <c r="T12" s="1">
+        <v>341000</v>
+      </c>
+      <c r="U12" s="1">
+        <v>6680</v>
+      </c>
+      <c r="V12" s="1">
+        <v>37000</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0</v>
+      </c>
+      <c r="X12" s="1">
+        <v>660000</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>292000</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>2195</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>593000</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>5780</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>19900</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>12000</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1">
+        <v>567</v>
+      </c>
+      <c r="D13" s="1">
+        <v>258000</v>
+      </c>
+      <c r="E13" s="1">
+        <v>492400</v>
+      </c>
+      <c r="F13" s="1">
+        <v>161300</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3000</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>6400000</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1350000</v>
+      </c>
+      <c r="K13" s="1">
+        <v>12066</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1767</v>
+      </c>
+      <c r="M13" s="1">
+        <v>3480000</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2400000</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>8330</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0</v>
+      </c>
+      <c r="U13" s="1">
+        <v>4580</v>
+      </c>
+      <c r="V13" s="1">
+        <v>92000</v>
+      </c>
+      <c r="W13" s="1">
+        <v>0</v>
+      </c>
+      <c r="X13" s="1">
+        <v>705000</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>168000</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>1144</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>376000</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>3270</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>7200</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>18000</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1">
+        <v>579</v>
+      </c>
+      <c r="D14" s="1">
+        <v>212000</v>
+      </c>
+      <c r="E14" s="1">
+        <v>499300</v>
+      </c>
+      <c r="F14" s="1">
+        <v>216000</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6000</v>
+      </c>
+      <c r="H14" s="1">
+        <v>10000</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2050000</v>
+      </c>
+      <c r="J14" s="1">
+        <v>11380000</v>
+      </c>
+      <c r="K14" s="1">
+        <v>3618</v>
+      </c>
+      <c r="L14" s="1">
+        <v>471</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1370000</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>440000</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <v>25630</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0</v>
+      </c>
+      <c r="U14" s="1">
+        <v>3710</v>
+      </c>
+      <c r="V14" s="1">
+        <v>269000</v>
+      </c>
+      <c r="W14" s="1">
+        <v>0</v>
+      </c>
+      <c r="X14" s="1">
+        <v>733000</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>270000</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>1031</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>481000</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>3120</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>4100</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1">
+        <v>559</v>
+      </c>
+      <c r="D15" s="1">
+        <v>302000</v>
+      </c>
+      <c r="E15" s="1">
+        <v>490500</v>
+      </c>
+      <c r="F15" s="1">
+        <v>107000</v>
+      </c>
+      <c r="G15" s="1">
+        <v>240000</v>
+      </c>
+      <c r="H15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2730000</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1530000</v>
+      </c>
+      <c r="K15" s="1">
+        <v>4987</v>
+      </c>
+      <c r="L15" s="1">
+        <v>750</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1430000</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>580000</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>1900</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1">
+        <v>2180</v>
+      </c>
+      <c r="T15" s="1">
+        <v>73000</v>
+      </c>
+      <c r="U15" s="1">
+        <v>8820</v>
+      </c>
+      <c r="V15" s="1">
+        <v>46000</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0</v>
+      </c>
+      <c r="X15" s="1">
+        <v>809000</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>592000</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>1343</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>1233000</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>7810</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>9400</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>7000</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>4543</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3000</v>
+      </c>
+      <c r="F16" s="1">
+        <v>60000</v>
+      </c>
+      <c r="G16" s="1">
+        <v>25000</v>
+      </c>
+      <c r="H16" s="1">
+        <v>17810000</v>
+      </c>
+      <c r="I16" s="1">
+        <v>540000</v>
+      </c>
+      <c r="J16" s="1">
+        <v>850000</v>
+      </c>
+      <c r="K16" s="1">
+        <v>979</v>
+      </c>
+      <c r="L16" s="1">
+        <v>317</v>
+      </c>
+      <c r="M16" s="1">
+        <v>2910000</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>460000</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>127700</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <v>1580</v>
+      </c>
+      <c r="T16" s="1">
+        <v>49000</v>
+      </c>
+      <c r="U16" s="1">
+        <v>430</v>
+      </c>
+      <c r="V16" s="1">
+        <v>7000</v>
+      </c>
+      <c r="W16" s="1">
+        <v>0</v>
+      </c>
+      <c r="X16" s="1">
+        <v>211000</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>12000</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>17</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>26000</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>250</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>100</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>4000</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F17" s="1">
+        <v>63000</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1200000</v>
+      </c>
+      <c r="I17" s="1">
+        <v>280000</v>
+      </c>
+      <c r="J17" s="1">
+        <v>250000</v>
+      </c>
+      <c r="K17" s="1">
+        <v>890</v>
+      </c>
+      <c r="L17" s="1">
+        <v>168</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1680000</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>260000</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>183500</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+      <c r="U17" s="1">
+        <v>460</v>
+      </c>
+      <c r="V17" s="1">
+        <v>11000</v>
+      </c>
+      <c r="W17" s="1">
+        <v>0</v>
+      </c>
+      <c r="X17" s="1">
+        <v>212000</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>12000</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>107</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>24000</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>170</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>300</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1">
+        <v>89</v>
+      </c>
+      <c r="D18" s="1">
+        <v>11000</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3300</v>
+      </c>
+      <c r="F18" s="1">
+        <v>228000</v>
+      </c>
+      <c r="G18" s="1">
+        <v>27000</v>
+      </c>
+      <c r="H18" s="1">
+        <v>260000</v>
+      </c>
+      <c r="I18" s="1">
+        <v>310000</v>
+      </c>
+      <c r="J18" s="1">
+        <v>730000</v>
+      </c>
+      <c r="K18" s="1">
+        <v>665</v>
+      </c>
+      <c r="L18" s="1">
+        <v>334</v>
+      </c>
+      <c r="M18" s="1">
+        <v>3670000</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>200000</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>8700</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1">
+        <v>100</v>
+      </c>
+      <c r="T18" s="1">
+        <v>5000</v>
+      </c>
+      <c r="U18" s="1">
+        <v>260</v>
+      </c>
+      <c r="V18" s="1">
+        <v>5000</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0</v>
+      </c>
+      <c r="X18" s="1">
+        <v>358000</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>27000</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>78</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>22000</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>150</v>
+      </c>
+      <c r="AD18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1">
+        <v>191</v>
+      </c>
+      <c r="D19" s="1">
+        <v>291000</v>
+      </c>
+      <c r="E19" s="1">
+        <v>52600</v>
+      </c>
+      <c r="F19" s="1">
+        <v>51000</v>
+      </c>
+      <c r="G19" s="1">
+        <v>17000</v>
+      </c>
+      <c r="H19" s="1">
+        <v>95000000</v>
+      </c>
+      <c r="I19" s="1">
+        <v>194000</v>
+      </c>
+      <c r="J19" s="1">
+        <v>34250000</v>
+      </c>
+      <c r="K19" s="1">
+        <v>17525</v>
+      </c>
+      <c r="L19" s="1">
+        <v>7110</v>
+      </c>
+      <c r="M19" s="1">
+        <v>10170000</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2530000</v>
+      </c>
+      <c r="P19" s="1">
+        <v>705800</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1900</v>
+      </c>
+      <c r="R19" s="1">
+        <v>10000</v>
+      </c>
+      <c r="S19" s="1">
+        <v>510</v>
+      </c>
+      <c r="T19" s="1">
+        <v>33000</v>
+      </c>
+      <c r="U19" s="1">
+        <v>6540</v>
+      </c>
+      <c r="V19" s="1">
+        <v>6000</v>
+      </c>
+      <c r="W19" s="1">
+        <v>0</v>
+      </c>
+      <c r="X19" s="1">
+        <v>352000</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>21000</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>14283</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>497000</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>5300</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>36100</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>79000</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1">
+        <v>175</v>
+      </c>
+      <c r="D20" s="1">
+        <v>286000</v>
+      </c>
+      <c r="E20" s="1">
+        <v>58200</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>27000</v>
+      </c>
+      <c r="H20" s="1">
+        <v>20000</v>
+      </c>
+      <c r="I20" s="1">
+        <v>900000</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2250000</v>
+      </c>
+      <c r="K20" s="1">
+        <v>5542</v>
+      </c>
+      <c r="L20" s="1">
+        <v>790</v>
+      </c>
+      <c r="M20" s="1">
+        <v>6780000</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>70000</v>
+      </c>
+      <c r="P20" s="1">
+        <v>34300</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+      <c r="S20" s="1">
+        <v>100</v>
+      </c>
+      <c r="T20" s="1">
+        <v>16000</v>
+      </c>
+      <c r="U20" s="1">
+        <v>2940</v>
+      </c>
+      <c r="V20" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W20" s="1">
+        <v>0</v>
+      </c>
+      <c r="X20" s="1">
+        <v>372000</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>26000</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>105</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>249000</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>8190</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>32000</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>68000</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1">
+        <v>165</v>
+      </c>
+      <c r="D21" s="1">
+        <v>260000</v>
+      </c>
+      <c r="E21" s="1">
+        <v>44000</v>
+      </c>
+      <c r="F21" s="1">
+        <v>38000</v>
+      </c>
+      <c r="G21" s="1">
+        <v>110000</v>
+      </c>
+      <c r="H21" s="1">
+        <v>54050000</v>
+      </c>
+      <c r="I21" s="1">
+        <v>2580000</v>
+      </c>
+      <c r="J21" s="1">
+        <v>21960000</v>
+      </c>
+      <c r="K21" s="1">
+        <v>8435</v>
+      </c>
+      <c r="L21" s="1">
+        <v>4774</v>
+      </c>
+      <c r="M21" s="1">
+        <v>5700000</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>1630000</v>
+      </c>
+      <c r="P21" s="1">
+        <v>186700</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>23600</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
+      <c r="U21" s="1">
+        <v>17920</v>
+      </c>
+      <c r="V21" s="1">
+        <v>10000</v>
+      </c>
+      <c r="W21" s="1">
+        <v>0</v>
+      </c>
+      <c r="X21" s="1">
+        <v>150000</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>14000</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>634</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>241000</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>6720</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>67500</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>49000</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1">
+        <v>208</v>
+      </c>
+      <c r="D22" s="1">
+        <v>204000</v>
+      </c>
+      <c r="E22" s="1">
+        <v>134200</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2795000</v>
+      </c>
+      <c r="H22" s="1">
+        <v>150000</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2070000</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1550000</v>
+      </c>
+      <c r="K22" s="1">
+        <v>8672</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1547</v>
+      </c>
+      <c r="M22" s="1">
+        <v>6360000</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>260000</v>
+      </c>
+      <c r="P22" s="1">
+        <v>32300</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>3900</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0</v>
+      </c>
+      <c r="S22" s="1">
+        <v>3550</v>
+      </c>
+      <c r="T22" s="1">
+        <v>5000</v>
+      </c>
+      <c r="U22" s="1">
+        <v>340</v>
+      </c>
+      <c r="V22" s="1">
+        <v>9000</v>
+      </c>
+      <c r="W22" s="1">
+        <v>250000</v>
+      </c>
+      <c r="X22" s="1">
+        <v>363000</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>27000</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>45</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>240000</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>360</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>240000</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>59000</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1">
+        <v>112</v>
+      </c>
+      <c r="D23" s="1">
+        <v>226000</v>
+      </c>
+      <c r="E23" s="1">
+        <v>19300</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G23" s="1">
+        <v>27000</v>
+      </c>
+      <c r="H23" s="1">
+        <v>90000</v>
+      </c>
+      <c r="I23" s="1">
+        <v>500000</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1920000</v>
+      </c>
+      <c r="K23" s="1">
+        <v>8100</v>
+      </c>
+      <c r="L23" s="1">
+        <v>844</v>
+      </c>
+      <c r="M23" s="1">
+        <v>6520000</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>70000</v>
+      </c>
+      <c r="P23" s="1">
+        <v>12400</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <v>2000</v>
+      </c>
+      <c r="S23" s="1">
+        <v>90</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
+        <v>860</v>
+      </c>
+      <c r="V23" s="1">
+        <v>11000</v>
+      </c>
+      <c r="W23" s="1">
+        <v>0</v>
+      </c>
+      <c r="X23" s="1">
+        <v>235000</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>27000</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>79</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>190000</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>1840</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>22600</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>118000</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>